<commit_message>
Provider relief increase based on monthly personal income
</commit_message>
<xml_diff>
--- a/results/09-2021/09-2021_comparison_deflators.xlsx
+++ b/results/09-2021/09-2021_comparison_deflators.xlsx
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1885</v>
+        <v>0.1884</v>
       </c>
       <c r="E4" t="n">
         <v>0.0739</v>
@@ -644,13 +644,13 @@
         <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0149</v>
+        <v>0.0215</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0314</v>
+        <v>0.131</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4518</v>
+        <v>0.2764</v>
       </c>
       <c r="F5" t="n">
         <v>-0.0291</v>
@@ -659,7 +659,7 @@
         <v>-0.0331</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0846</v>
+        <v>-0.0847</v>
       </c>
       <c r="I5" t="n">
         <v>-0.0524</v>
@@ -671,7 +671,7 @@
         <v>-0.3977</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1381</v>
+        <v>-0.1382</v>
       </c>
       <c r="M5" t="n">
         <v>-0.0277</v>
@@ -685,37 +685,37 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0156</v>
+        <v>-0.024</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0211</v>
+        <v>-0.0296</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.0166</v>
+        <v>-0.025</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0518</v>
+        <v>-0.0515</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0493</v>
+        <v>-0.0491</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0553</v>
+        <v>-0.055</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0403</v>
+        <v>-0.0401</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0726</v>
+        <v>-0.0723</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0683</v>
+        <v>-0.068</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0429</v>
+        <v>-0.0427</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0348</v>
+        <v>-0.0346</v>
       </c>
     </row>
     <row r="7">
@@ -726,37 +726,37 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2564</v>
+        <v>-0.2563</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0161</v>
+        <v>-0.0177</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0135</v>
+        <v>-0.0188</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1718</v>
+        <v>0.1253</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2688</v>
+        <v>0.2236</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.0757</v>
+        <v>-0.0851</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.1076</v>
+        <v>-0.1174</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1647</v>
+        <v>-0.1602</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1859</v>
+        <v>-0.182</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0426</v>
+        <v>0.043</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1283</v>
+        <v>0.1276</v>
       </c>
     </row>
     <row r="8">
@@ -767,37 +767,37 @@
         <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2688</v>
+        <v>-0.2721</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1929</v>
+        <v>-0.196</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1674</v>
+        <v>-0.1689</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1227</v>
+        <v>-0.1238</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.396</v>
+        <v>-0.3971</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.3017</v>
+        <v>-0.303</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.2013</v>
+        <v>-0.2026</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.0776</v>
+        <v>-0.0789</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0344</v>
+        <v>-0.0342</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0176</v>
+        <v>-0.0175</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0018</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="9">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5004</v>
+        <v>0.5001</v>
       </c>
       <c r="E9" t="n">
         <v>0.0354</v>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4837</v>
+        <v>0.4835</v>
       </c>
       <c r="E10" t="n">
         <v>0.1057</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0099</v>
+        <v>0.0102</v>
       </c>
       <c r="D11" t="n">
         <v>0.0053</v>
@@ -931,10 +931,10 @@
         <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.6158</v>
+        <v>-0.5948</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.0497</v>
+        <v>-1.0492</v>
       </c>
       <c r="E12" t="n">
         <v>-0.5506</v>
@@ -943,7 +943,7 @@
         <v>-1.2909</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.5127</v>
+        <v>-0.5319</v>
       </c>
       <c r="H12" t="n">
         <v>-0.2061</v>
@@ -972,37 +972,37 @@
         <v>14</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3712</v>
+        <v>0.3833</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3515</v>
+        <v>0.2726</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1341</v>
+        <v>-0.1238</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.0908</v>
+        <v>-0.0875</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1118</v>
+        <v>-0.1085</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1027</v>
+        <v>-0.0991</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0596</v>
+        <v>-0.0592</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0484</v>
+        <v>-0.048</v>
       </c>
       <c r="K13" t="n">
         <v>-0.6156</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.6542</v>
+        <v>-0.6506</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.3085</v>
+        <v>-0.3081</v>
       </c>
     </row>
     <row r="14">
@@ -1013,34 +1013,34 @@
         <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1723</v>
+        <v>0.1724</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.9051</v>
+        <v>-0.7572</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.0885</v>
+        <v>-1.1114</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.9873</v>
+        <v>-0.9955</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.4772</v>
+        <v>-1.4852</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.0265</v>
+        <v>-1.0685</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.4125</v>
+        <v>-0.4401</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.4044</v>
+        <v>-0.4047</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.3141</v>
+        <v>-0.321</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.1478</v>
+        <v>-0.1744</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1054,37 +1054,37 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.8281</v>
+        <v>-2.7628</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.0739</v>
+        <v>-1.9883</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.904</v>
+        <v>-2.9886</v>
       </c>
       <c r="F15" t="n">
-        <v>-2.1373</v>
+        <v>-2.1825</v>
       </c>
       <c r="G15" t="n">
-        <v>-3.6794</v>
+        <v>-3.7821</v>
       </c>
       <c r="H15" t="n">
-        <v>-2.0278</v>
+        <v>-2.0184</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.6562</v>
+        <v>-1.6445</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.7535</v>
+        <v>-1.7017</v>
       </c>
       <c r="K15" t="n">
-        <v>-2.821</v>
+        <v>-2.8308</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.1663</v>
+        <v>-1.1846</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.577</v>
+        <v>-0.5898</v>
       </c>
     </row>
     <row r="16">
@@ -1095,7 +1095,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>22731.4</v>
+        <v>22741</v>
       </c>
       <c r="D16" t="n">
         <v>23334.3</v>
@@ -1136,13 +1136,13 @@
         <v>14</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5297</v>
+        <v>0.5458</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0562</v>
+        <v>0.2185</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5218</v>
+        <v>0.3464</v>
       </c>
       <c r="F17" t="n">
         <v>0.0379</v>
@@ -1151,16 +1151,16 @@
         <v>0.1914</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1933</v>
+        <v>0.1932</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2092</v>
+        <v>0.2091</v>
       </c>
       <c r="J17" t="n">
         <v>0.2159</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.2325</v>
+        <v>-0.2326</v>
       </c>
       <c r="L17" t="n">
         <v>0.0053</v>
@@ -1218,37 +1218,37 @@
         <v>14</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.0495</v>
+        <v>-1.0494</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0003</v>
+        <v>0.0464</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.2174</v>
+        <v>-1.2305</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0114</v>
+        <v>0.0112</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0308</v>
+        <v>-0.0313</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0467</v>
+        <v>-0.0333</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.0355</v>
+        <v>-0.0353</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.051</v>
+        <v>-0.0348</v>
       </c>
       <c r="K19" t="n">
-        <v>-1.0902</v>
+        <v>-1.0901</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.0006</v>
+        <v>-0.0005</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.0161</v>
+        <v>-0.0307</v>
       </c>
     </row>
     <row r="20">
@@ -1259,19 +1259,19 @@
         <v>14</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.2712</v>
+        <v>-0.2711</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.2693</v>
+        <v>-1.2688</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.2748</v>
+        <v>-0.2747</v>
       </c>
       <c r="F20" t="n">
         <v>-0.028</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.026</v>
+        <v>-1.0259</v>
       </c>
       <c r="H20" t="n">
         <v>-0.0282</v>
@@ -1300,13 +1300,13 @@
         <v>14</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.709</v>
+        <v>-0.7397</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3351</v>
+        <v>0.1726</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.0136</v>
+        <v>0.1617</v>
       </c>
       <c r="F21" t="n">
         <v>0.331</v>
@@ -1324,13 +1324,13 @@
         <v>-0.2683</v>
       </c>
       <c r="K21" t="n">
-        <v>0.183</v>
+        <v>0.1831</v>
       </c>
       <c r="L21" t="n">
         <v>-0.0562</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.1339</v>
+        <v>-0.1338</v>
       </c>
     </row>
     <row r="22">
@@ -1341,7 +1341,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.0132</v>
+        <v>-0.014</v>
       </c>
       <c r="D22" t="n">
         <v>-0.0289</v>
@@ -1362,7 +1362,7 @@
         <v>-0.02</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.0223</v>
+        <v>-0.0222</v>
       </c>
       <c r="K22" t="n">
         <v>-0.0233</v>
@@ -1382,37 +1382,37 @@
         <v>14</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2168</v>
+        <v>0.1964</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.0041</v>
+        <v>-0.0326</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1551</v>
+        <v>0.1275</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0163</v>
+        <v>0.0049</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.0785</v>
+        <v>-0.0708</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1311</v>
+        <v>0.1439</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1273</v>
+        <v>0.1399</v>
       </c>
       <c r="J23" t="n">
-        <v>0.2062</v>
+        <v>0.2038</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1939</v>
+        <v>0.1915</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.0182</v>
+        <v>-0.0178</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0085</v>
+        <v>0.0084</v>
       </c>
     </row>
     <row r="24">
@@ -1423,37 +1423,37 @@
         <v>14</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.1693</v>
+        <v>-0.0802</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.2279</v>
+        <v>-0.1476</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.182</v>
+        <v>-0.1458</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.1537</v>
+        <v>-0.1149</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.211</v>
+        <v>-0.1726</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.1659</v>
+        <v>-0.128</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.1707</v>
+        <v>-0.1333</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.1414</v>
+        <v>-0.1044</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0676</v>
+        <v>-0.0698</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.0316</v>
+        <v>-0.0311</v>
       </c>
       <c r="M24" t="n">
-        <v>-0.0192</v>
+        <v>-0.0188</v>
       </c>
     </row>
     <row r="25">
@@ -1464,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0175</v>
+        <v>0.0178</v>
       </c>
       <c r="D25" t="n">
         <v>0.0101</v>
@@ -1587,37 +1587,37 @@
         <v>14</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.2283</v>
+        <v>-0.2286</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.2049</v>
+        <v>-0.2414</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.0568</v>
+        <v>-0.0821</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.0988</v>
+        <v>-0.119</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.2135</v>
+        <v>-0.2302</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.0711</v>
+        <v>-0.077</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.0399</v>
+        <v>-0.0404</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.0365</v>
+        <v>-0.0391</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.0223</v>
+        <v>-0.0247</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.0119</v>
+        <v>-0.0089</v>
       </c>
       <c r="M28" t="n">
-        <v>-0.0056</v>
+        <v>-0.0042</v>
       </c>
     </row>
     <row r="29">
@@ -1713,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1751,13 +1751,13 @@
         <v>41</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.0066</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>0.1623</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>-0.1753</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1792,37 +1792,37 @@
         <v>41</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>-0.0084</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>-0.0085</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>-0.0083</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="34">
@@ -1833,37 +1833,37 @@
         <v>41</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>-0.0338</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>-0.0323</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>-0.0465</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>-0.0452</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>-0.0094</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>-0.0098</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>0.0045</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>0.0039</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
     </row>
     <row r="35">
@@ -1874,37 +1874,37 @@
         <v>41</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>-0.0033</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>-0.0031</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>-0.0015</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>-0.0013</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>-0.0013</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>-0.0013</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="36">
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1997,7 +1997,7 @@
         <v>41</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -2038,10 +2038,10 @@
         <v>41</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>0.021</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>-0.0192</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -2079,37 +2079,37 @@
         <v>41</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>-0.0789</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>0.0103</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>0.0034</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>0.0033</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>0.0037</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>0.0035</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="41">
@@ -2123,31 +2123,31 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>0.148</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>-0.0229</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>-0.0082</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>-0.008</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>-0.042</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>-0.0276</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>-0.007</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>-0.0266</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
@@ -2161,37 +2161,37 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.0653</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>0.0855</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>-0.0846</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>-0.0452</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>-0.1027</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>0.0094</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>0.0117</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>0.0518</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>-0.0097</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>-0.0183</v>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>-0.0128</v>
       </c>
     </row>
     <row r="43">
@@ -2202,7 +2202,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -2243,13 +2243,13 @@
         <v>41</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>0.0161</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>0.1623</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>-0.1753</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -2325,37 +2325,37 @@
         <v>41</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>0.0461</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>-0.0132</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>-0.062</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>0.0134</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>0.0162</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="L46" t="n">
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>-0.0145</v>
       </c>
     </row>
     <row r="47">
@@ -2366,10 +2366,10 @@
         <v>41</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>0.0006</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -2407,13 +2407,13 @@
         <v>41</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>-0.0307</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>-0.1625</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>0.1753</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -2448,7 +2448,7 @@
         <v>41</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>-0.0008</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -2489,37 +2489,37 @@
         <v>41</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>-0.0204</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>-0.0285</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>-0.0276</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>-0.0114</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>0.0076</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>0.0128</v>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>0.0126</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>-0.0023</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>-0.0024</v>
       </c>
       <c r="L50" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="M50" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
     </row>
     <row r="51">
@@ -2530,37 +2530,37 @@
         <v>41</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>0.0892</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>0.0803</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>0.0362</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>0.0389</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>0.0384</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>0.0379</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>0.0374</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>-0.0023</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="M51" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="52">
@@ -2571,7 +2571,7 @@
         <v>41</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -2694,37 +2694,37 @@
         <v>41</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>-0.0365</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>-0.0253</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>-0.0202</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>-0.0167</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>-0.0059</v>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>-0.0026</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>-0.0024</v>
       </c>
       <c r="L55" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="M55" t="n">
-        <v>0</v>
+        <v>0.0014</v>
       </c>
     </row>
     <row r="56">

</xml_diff>